<commit_message>
se trabaja en inspeccion por equipos EPP, se trabaja en hacerlo por excel y por link de publico en /inspeccion
</commit_message>
<xml_diff>
--- a/public/resources/plantilla-subir-colaboradores.xlsx
+++ b/public/resources/plantilla-subir-colaboradores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESARROLLADOR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESARROLLADOR\Documents\desarrollo\tisog-claro\claro-altura\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082BEF60-740A-4106-8CEB-FEE70913F3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F646F744-D77D-488B-90DB-0BC18AA32F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4F0692C0-6631-4375-AACD-9873D1420926}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="empleados" sheetId="1" r:id="rId1"/>
     <sheet name="valores" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">empleados!$A$1:$F$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Nombres</t>
   </si>
@@ -37,38 +40,104 @@
     <t># Documento</t>
   </si>
   <si>
+    <t xml:space="preserve">[obligatorio] </t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Tipo Documento</t>
+  </si>
+  <si>
+    <t>TipoDoc</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Ciudades</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
+  </si>
+  <si>
+    <t>Bucaramanga</t>
+  </si>
+  <si>
+    <t>Cali</t>
+  </si>
+  <si>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Cúcuta</t>
+  </si>
+  <si>
+    <t>Florencia</t>
+  </si>
+  <si>
+    <t>Ibagué</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>Montería</t>
+  </si>
+  <si>
+    <t>Neiva</t>
+  </si>
+  <si>
+    <t>Pasto</t>
+  </si>
+  <si>
+    <t>Pereira</t>
+  </si>
+  <si>
+    <t>Santa Marta</t>
+  </si>
+  <si>
+    <t>Sincelejo</t>
+  </si>
+  <si>
+    <t>Tunja</t>
+  </si>
+  <si>
+    <t>Valledupar</t>
+  </si>
+  <si>
+    <t>Villavicencio</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t>Yopal</t>
+  </si>
+  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
-    <t xml:space="preserve">[obligatorio] </t>
-  </si>
-  <si>
-    <t>Indefinido</t>
-  </si>
-  <si>
-    <t>Término fijo</t>
-  </si>
-  <si>
-    <t>Por obra o labor</t>
-  </si>
-  <si>
-    <t>Prácticas laborales</t>
-  </si>
-  <si>
-    <t>Temporal</t>
-  </si>
-  <si>
-    <t>Medio tiempo</t>
-  </si>
-  <si>
-    <t>TipoContrato</t>
+    <t xml:space="preserve">[opcional] </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +173,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF020817"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -126,7 +201,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -146,7 +221,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,11 +229,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Estilo 2" xfId="1" xr:uid="{26E67B80-E42F-4495-A350-3887F7438A2E}"/>
@@ -474,26 +552,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6523FF5B-0B1D-4E6A-AD8E-A920C4C9386C}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,43 +581,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E713202-CA2C-4A85-AA96-06142AACD8A1}">
           <x14:formula1>
             <xm:f>valores!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F800</xm:sqref>
+          <xm:sqref>H4:H800</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{527F85AE-91FC-4E45-BFA4-7A25C2AB740A}">
+          <x14:formula1>
+            <xm:f>valores!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C1032</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BDD455E-904C-4EA4-B71C-58F4C79B9DDA}">
+          <x14:formula1>
+            <xm:f>valores!$B$2:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -547,50 +647,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46139D6B-7EB2-44E8-BBD5-967006769924}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>